<commit_message>
Function GEN SGDC completed. Updating function GEN StarECO and in progress diagram for GEN StarECO.
</commit_message>
<xml_diff>
--- a/python/ecolist.xlsx
+++ b/python/ecolist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://questglobalo365-my.sharepoint.com/personal/duc_luong_quest-global_com/Documents/Desktop/Synapse_training/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="92" documentId="8_{3765CC2E-D01C-4120-9584-3C31B1915DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99FC0F9F-DE90-4847-A50A-0250D5F7ED56}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{3765CC2E-D01C-4120-9584-3C31B1915DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F469EF3-70D2-417C-9FA3-B950AC39B8B6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16470" yWindow="1695" windowWidth="15375" windowHeight="7965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ecolist" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>No</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>HLB18_MAIN.path.to.clock0</t>
+  </si>
+  <si>
+    <t>OnlyScanMode</t>
   </si>
 </sst>
 </file>
@@ -1146,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,9 +1164,10 @@
     <col min="5" max="6" width="9.140625" style="3"/>
     <col min="7" max="7" width="4.5703125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1188,8 +1192,11 @@
       <c r="H1" s="7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1212,7 +1219,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1232,7 +1239,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1255,7 +1262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1277,8 +1284,11 @@
       <c r="G5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1301,7 +1311,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1327,7 +1337,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Update starECO: reset complete
</commit_message>
<xml_diff>
--- a/python/ecolist.xlsx
+++ b/python/ecolist.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>SGDC:</t>
   </si>
@@ -105,7 +105,7 @@
     <t>HLB18_MAIN.path.to.testmode1</t>
   </si>
   <si>
-    <t>contraint</t>
+    <t>constraint</t>
   </si>
   <si>
     <t>HLB18_MAIN.testmode2</t>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>reset</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>HLB18_MAIN.reset1</t>
@@ -125,7 +128,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +138,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -165,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -297,6 +306,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFc6c6c6"/>
       </left>
@@ -335,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -376,16 +392,22 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
@@ -397,26 +419,38 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,199 +760,199 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="27" width="5.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="32" width="5.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="16" width="36.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="15" width="9.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="27" width="9.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="9.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="33" width="9.147857142857141" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="16" width="9.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="4.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="16" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="4.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="18" width="12.290714285714287" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="16" width="14.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="G1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="20">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="25">
         <v>200</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="24"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="25">
+      <c r="G2" s="24"/>
+      <c r="H2" s="26"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="A3" s="27">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="26"/>
-      <c r="E3" s="24" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="26" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="23">
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="25">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="28" t="s">
         <v>27</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="30">
         <v>100</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="26">
+      <c r="G4" s="25"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="29">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="26" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="27">
         <v>1</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="23" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="26">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="29">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="27">
         <v>0</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="24"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="23">
+      <c r="G6" s="24"/>
+      <c r="H6" s="26"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="25">
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="25">
         <v>0</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="28" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="22"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="23">
+      <c r="G7" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="24"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="25">
         <v>7</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="22" t="s">
+      <c r="B8" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="29">
         <v>1</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="26" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="21"/>
+      <c r="H8" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -936,15 +970,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="10.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="10.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="17" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="18" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="18" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1050,7 +1084,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="14"/>
-      <c r="B8" s="3"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -1061,7 +1095,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="14"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>

</xml_diff>